<commit_message>
Changed Test Case Name in Xcel sheet
</commit_message>
<xml_diff>
--- a/ShellTest/src/main/java/com/Shell/qa/TestData/POMTestDataSheet.xlsx
+++ b/ShellTest/src/main/java/com/Shell/qa/TestData/POMTestDataSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sb49849.IND\Desktop\ShellTest\src\main\java\com\Shell\qa\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sb49849.IND\git\Framework\ShellTest\src\main\java\com\Shell\qa\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCB25AC-8F89-490A-813B-61A2269F3B80}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5AF641-9ACB-466A-8259-9A497F224057}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{3E99FE3A-74EA-45CD-8159-3B7EB1DC3932}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{3E99FE3A-74EA-45CD-8159-3B7EB1DC3932}"/>
   </bookViews>
   <sheets>
     <sheet name="POM TestCases" sheetId="1" r:id="rId1"/>
@@ -42,12 +42,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>LoginPageTest</t>
-  </si>
-  <si>
-    <t>HomePageTest</t>
-  </si>
-  <si>
     <t>UserName</t>
   </si>
   <si>
@@ -58,6 +52,12 @@
   </si>
   <si>
     <t>HiP3rf0rm@ncefuel</t>
+  </si>
+  <si>
+    <t>TC02_HomePageTest</t>
+  </si>
+  <si>
+    <t>TC01_LoginPageTest</t>
   </si>
 </sst>
 </file>
@@ -490,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FE0DFCA-6B94-430A-AA2D-9F73C46EC2B9}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,7 +510,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
@@ -539,9 +539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C18B3DD0-C95F-441D-80BB-1B5EE397BE81}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -551,37 +549,37 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B6" s="4"/>
     </row>

</xml_diff>